<commit_message>
add LeaveRoundaboutAsUturn / LeaveRoundaboutAsUturnCC arrow, but cannot recognize them by 8x8 image.
</commit_message>
<xml_diff>
--- a/GoogleMap_Arrow_Recognize/PatternRecognize/workdir/8x8_image_recognize.xlsx
+++ b/GoogleMap_Arrow_Recognize/PatternRecognize/workdir/8x8_image_recognize.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\GitHub\Garminuino\GoogleMap_Arrow_Recognize\PatternRecognize\workdir\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570D0481-1DEF-42AC-AE75-3BC69B837FF5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{1015E351-78D5-46F2-8C4B-26B800CCCDFB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="lookup" sheetId="4" r:id="rId1"/>
     <sheet name="split workspace" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="111">
   <si>
     <t>SharpRight</t>
   </si>
@@ -161,114 +155,6 @@
   </si>
   <si>
     <t>LeaveRoundaboutSharpRightCC</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutAsDirection</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutAsDirectionCC</t>
-  </si>
-  <si>
-    <t>Arrivals.png</t>
-  </si>
-  <si>
-    <t>ArrivalsLeft.png</t>
-  </si>
-  <si>
-    <t>ArrivalsRight.png</t>
-  </si>
-  <si>
-    <t>Convergence.png</t>
-  </si>
-  <si>
-    <t>EasyLeft.png</t>
-  </si>
-  <si>
-    <t>EasyRight.png</t>
-  </si>
-  <si>
-    <t>GoTo.png</t>
-  </si>
-  <si>
-    <t>KeepLeft.png</t>
-  </si>
-  <si>
-    <t>KeepRight.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundabout.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutAsDirection.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutAsDirectionCC.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutCC.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutEasyLeft.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutEasyLeftCC.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutEasyRight.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutEasyRightCC.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutLeft.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutLeftCC.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutRight.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutRightCC.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutSharpLeft.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutSharpLeftCC.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutSharpRight.png</t>
-  </si>
-  <si>
-    <t>LeaveRoundaboutSharpRightCC.png</t>
-  </si>
-  <si>
-    <t>Left.png</t>
-  </si>
-  <si>
-    <t>LeftDown.png</t>
-  </si>
-  <si>
-    <t>LeftToLeave.png</t>
-  </si>
-  <si>
-    <t>Right.png</t>
-  </si>
-  <si>
-    <t>RightDown.png</t>
-  </si>
-  <si>
-    <t>RightToLeave.png</t>
-  </si>
-  <si>
-    <t>SharpLeft.png</t>
-  </si>
-  <si>
-    <t>SharpRight.png</t>
-  </si>
-  <si>
-    <t>Straight.png</t>
   </si>
   <si>
     <t>4046528486445154304</t>
@@ -448,13 +334,40 @@
   <si>
     <t>8x8_right_dw</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2916125187146266624</t>
+  </si>
+  <si>
+    <t>8668387462071461888</t>
+  </si>
+  <si>
+    <t>4052175854055995392</t>
+  </si>
+  <si>
+    <t>8668422303588558848</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>LeaveRoundaboutAsUturn</t>
+  </si>
+  <si>
+    <t>LeaveRoundaboutAsUturnCC</t>
+  </si>
+  <si>
+    <t>LeaveRoundaboutStraight</t>
+  </si>
+  <si>
+    <t>LeaveRoundaboutStraightCC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -560,7 +473,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -612,7 +525,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -806,36 +719,36 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16357B61-2CFF-4045-A35E-2BAB2DBA03E8}">
-  <dimension ref="B1:E35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E35"/>
+      <selection activeCell="E37" sqref="E2:E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="30.875" customWidth="1"/>
-    <col min="3" max="4" width="27.375" customWidth="1"/>
+    <col min="2" max="2" width="30.90625" customWidth="1"/>
+    <col min="3" max="4" width="27.36328125" customWidth="1"/>
     <col min="5" max="5" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5">
       <c r="C1" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5">
       <c r="B2" t="s">
         <v>22</v>
       </c>
@@ -843,44 +756,44 @@
         <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>79</v>
+        <v>43</v>
       </c>
       <c r="E2" t="str">
         <f>B2&amp;"("&amp;C2&amp;"L,"&amp;D2&amp;"L),"</f>
         <v>Arrivals(1157442937613201408L,4046528486445154304L),</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E35" si="0">B3&amp;"("&amp;C3&amp;"L,"&amp;D3&amp;"L),"</f>
+        <f t="shared" ref="E3:E37" si="0">B3&amp;"("&amp;C3&amp;"L,"&amp;D3&amp;"L),"</f>
         <v>ArrivalsLeft(6372721067853220864L,6962811727307355648L),</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5">
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>82</v>
+        <v>46</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
         <v>ArrivalsRight(3899022579807051776L,291060571498928128L),</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -888,14 +801,14 @@
         <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
         <v>Convergence(5505712186103173120L,1168701902593477632L),</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -903,44 +816,44 @@
         <v>26</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v>EasyLeft(4629771062305364992L,8084009726888903680L),</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
         <v>EasyRight(289360692026306560L,2024482657668186112L),</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
         <v>GoTo(4521450452025344L,4565430246047744L),</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -948,29 +861,29 @@
         <v>27</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
         <v>KeepLeft(1157442799634484224L,6944586016205312000L),</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5">
       <c r="B10" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
         <v>KeepRight(1157442903121879040L,868077727617388544L),</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5">
       <c r="B11" t="s">
         <v>16</v>
       </c>
@@ -978,119 +891,119 @@
         <v>28</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundabout(433484693105016832L,2337403529502687232L),</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5">
       <c r="B12" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>102</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>LeaveRoundaboutAsDirection(1732773254121656320L,3474580302471376912L),</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+        <v>LeaveRoundaboutAsUturn(2916125187146266624L,8668387462071461888L),</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
       <c r="B13" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>LeaveRoundaboutAsDirectionCC(3476849762382647296L,3474544807983716368L),</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+        <v>LeaveRoundaboutAsUturnCC(4052175854055995392L,8668422303588558848L),</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
       <c r="B14" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutCC(54148887964819456L,583224982398961152L),</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5">
       <c r="B15" t="s">
         <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>98</v>
+        <v>62</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutEasyLeft(4037481515658380800L,18085043212652560L),</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5">
       <c r="B16" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutEasyLeftCC(6971713514041116160L,34907320997384208L),</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5">
       <c r="B17" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutEasyRight(1730512573871734784L,468031865528262688L),</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5">
       <c r="B18" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutEasyRightCC(3476849557575352320L,436299425423826976L),</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -1098,44 +1011,44 @@
         <v>29</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutLeft(4629806193894752256L,18278659459386380L),</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5">
       <c r="B20" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>107</v>
+        <v>71</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>108</v>
+        <v>72</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutLeftCC(4629771353129807872L,6841779608766647308L),</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5">
       <c r="B21" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>110</v>
+        <v>74</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutRight(868082327038860800L,8115098127117074496L),</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -1143,204 +1056,234 @@
         <v>30</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>111</v>
+        <v>75</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutRightCC(868082369943306240L,1159402266574912L),</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5">
       <c r="B23" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>112</v>
+        <v>76</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>113</v>
+        <v>77</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutSharpLeft(2318839477172174848L,36219191824400L),</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5">
       <c r="B24" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>115</v>
+        <v>79</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutSharpLeftCC(2318277354143150080L,2622824501374097432L),</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5">
       <c r="B25" t="s">
         <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>116</v>
+        <v>80</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>117</v>
+        <v>81</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutSharpRight(1799426286098332672L,6379498870348849184L),</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5">
       <c r="B26" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
         <v>LeaveRoundaboutSharpRightCC(1211698028973391872L,17850624385056L),</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5">
       <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>LeaveRoundaboutStraight(1732773254121656320L,3474580302471376912L),</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>LeaveRoundaboutStraightCC(3476849762382647296L,3474544807983716368L),</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E27" t="str">
+      <c r="C29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" t="str">
         <f t="shared" si="0"/>
         <v>Left(4629771061775042560L,34942496777962496L),</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="30" spans="2:5">
+      <c r="B30" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E28" t="str">
+      <c r="C30" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" t="str">
         <f t="shared" si="0"/>
         <v>LeftDown(19215401358983168L,15873530252230656L),</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="31" spans="2:5">
+      <c r="B31" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E29" t="str">
+      <c r="C31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" t="str">
         <f t="shared" si="0"/>
         <v>LeftToLeave(4665940630367375360L,2337429830863422464L),</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="32" spans="2:5">
+      <c r="B32" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" t="str">
+      <c r="C32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" t="str">
         <f t="shared" si="0"/>
         <v>Right(289360691897049088L,34986735951691776L),</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="33" spans="2:5">
+      <c r="B33" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E31" t="str">
+      <c r="C33" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" t="str">
         <f t="shared" si="0"/>
         <v>RightDown(1201647631466496L,15872886011330560L),</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="34" spans="2:5">
+      <c r="B34" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" t="str">
+      <c r="D34" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" t="str">
         <f t="shared" si="0"/>
         <v>RightToLeave(289360727672619008L,584456678972375040L),</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="35" spans="2:5">
+      <c r="B35" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E33" t="str">
+      <c r="C35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" t="str">
         <f t="shared" si="0"/>
         <v>SharpLeft(18085095220985856L,291665680040985600L),</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="36" spans="2:5">
+      <c r="B36" t="s">
         <v>0</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E34" t="str">
+      <c r="C36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E36" t="str">
         <f t="shared" si="0"/>
         <v>SharpRight(1130728323286016L,4638809098756833280L),</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="37" spans="2:5">
+      <c r="B37" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E35" t="str">
+      <c r="D37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E37" t="str">
         <f t="shared" si="0"/>
         <v>Straight(1157442765411848192L,1168701764477652992L),</v>
       </c>
@@ -1348,400 +1291,531 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2EB53A1-C38F-4A23-B940-452ADE1A2E08}">
-  <dimension ref="B2:D35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C35"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="3" width="32.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="32.125" customWidth="1"/>
+    <col min="2" max="3" width="32.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5">
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5">
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="D24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D25" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
+        <v>110</v>
+      </c>
+      <c r="E27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D35" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="B36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D29" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D33" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D35" t="s">
-        <v>78</v>
+      <c r="D36" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>